<commit_message>
data-mining: export excel as pdf
</commit_message>
<xml_diff>
--- a/data-mining/lab1/lab1.xlsx
+++ b/data-mining/lab1/lab1.xlsx
@@ -2,14 +2,14 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="26215"/>
-  <workbookPr autoCompressPictures="0"/>
+  <workbookPr checkCompatibility="1" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Drapegnik/Dropbox/bsu/vkiad/lab1/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Drapegnik/projects/bsu/data-mining/lab1/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="740" yWindow="460" windowWidth="24860" windowHeight="15540"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
   </externalReferences>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$A$47</definedName>
-    <definedName name="_xlnm.Extract" localSheetId="0">Sheet1!$C$2:$C$18</definedName>
+    <definedName name="_xlnm.Extract" localSheetId="0">Sheet1!$C$9:$C$18</definedName>
   </definedNames>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
@@ -52,7 +52,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -67,6 +67,12 @@
       <name val="Consolas"/>
       <family val="3"/>
       <charset val="204"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -150,7 +156,7 @@
           <c:order val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$G$4:$G$10</c:f>
+              <c:f>Sheet1!$F$2:$F$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -190,11 +196,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2117248512"/>
-        <c:axId val="2117245376"/>
+        <c:axId val="-2084829760"/>
+        <c:axId val="-2118500928"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2117248512"/>
+        <c:axId val="-2084829760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -204,7 +210,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2117245376"/>
+        <c:crossAx val="-2118500928"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -212,7 +218,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2117245376"/>
+        <c:axId val="-2118500928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -242,7 +248,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2117248512"/>
+        <c:crossAx val="-2084829760"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -310,7 +316,7 @@
           <c:order val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$H$4:$H$10</c:f>
+              <c:f>Sheet1!$G$2:$G$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -350,11 +356,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2117329120"/>
-        <c:axId val="2117331936"/>
+        <c:axId val="-2070230816"/>
+        <c:axId val="-2070456640"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2117329120"/>
+        <c:axId val="-2070230816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -364,7 +370,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2117331936"/>
+        <c:crossAx val="-2070456640"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -372,7 +378,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2117331936"/>
+        <c:axId val="-2070456640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -402,7 +408,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2117329120"/>
+        <c:crossAx val="-2070230816"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -671,11 +677,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2117378528"/>
-        <c:axId val="2117381360"/>
+        <c:axId val="-2145092064"/>
+        <c:axId val="-2075784192"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2117378528"/>
+        <c:axId val="-2145092064"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -685,7 +691,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2117381360"/>
+        <c:crossAx val="-2075784192"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -693,7 +699,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2117381360"/>
+        <c:axId val="-2075784192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -723,7 +729,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2117378528"/>
+        <c:crossAx val="-2145092064"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -744,16 +750,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>242887</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>123825</xdr:rowOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>319087</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>136524</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>1023937</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>1587500</xdr:colOff>
+      <xdr:row>60</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -774,16 +780,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>1619250</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>336550</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>152400</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>1600200</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -806,16 +812,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>333375</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>111125</xdr:rowOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>371475</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>638175</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>177800</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>1574800</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1417,248 +1423,252 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H47"/>
+  <dimension ref="A1:G47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q20" sqref="Q20"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="I43" sqref="I43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="6" max="6" width="12.83203125" customWidth="1"/>
-    <col min="7" max="7" width="25.6640625" customWidth="1"/>
+    <col min="1" max="1" width="4.33203125" customWidth="1"/>
+    <col min="2" max="2" width="5.6640625" customWidth="1"/>
+    <col min="3" max="3" width="8.1640625" customWidth="1"/>
+    <col min="5" max="5" width="16.1640625" customWidth="1"/>
+    <col min="6" max="6" width="17.5" customWidth="1"/>
+    <col min="7" max="7" width="22" customWidth="1"/>
     <col min="8" max="8" width="26.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1">
         <v>8</v>
       </c>
       <c r="B1" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>7</v>
       </c>
       <c r="B2" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C2">
+        <v>6</v>
+      </c>
+      <c r="D2">
+        <f>COUNTIF($A$1:$A$47,C2)</f>
+        <v>3</v>
+      </c>
+      <c r="E2">
+        <f>D2/SUM($D$1:$D$10)</f>
+        <v>8.5714285714285715E-2</v>
+      </c>
+      <c r="F2">
+        <f>SUM(D$2:D2)</f>
+        <v>3</v>
+      </c>
+      <c r="G2">
+        <f>SUM(E$2:E2)</f>
+        <v>8.5714285714285715E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>8</v>
       </c>
       <c r="B3" s="1">
         <v>3</v>
       </c>
-      <c r="D3" t="s">
-        <v>0</v>
-      </c>
-      <c r="E3" t="s">
-        <v>1</v>
-      </c>
-      <c r="F3" t="s">
-        <v>2</v>
-      </c>
-      <c r="G3" t="s">
-        <v>3</v>
-      </c>
-      <c r="H3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C3">
+        <v>7</v>
+      </c>
+      <c r="D3">
+        <f>COUNTIF($A$1:$A$47,C3)</f>
+        <v>11</v>
+      </c>
+      <c r="E3">
+        <f>D3/SUM($D$1:$D$10)</f>
+        <v>0.31428571428571428</v>
+      </c>
+      <c r="F3">
+        <f>SUM(D$2:D3)</f>
+        <v>14</v>
+      </c>
+      <c r="G3">
+        <f>SUM(E$2:E3)</f>
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>8</v>
       </c>
       <c r="B4" s="1">
         <v>4</v>
       </c>
+      <c r="C4">
+        <v>8</v>
+      </c>
       <c r="D4">
-        <v>6</v>
+        <f>COUNTIF($A$1:$A$47,C4)</f>
+        <v>9</v>
       </c>
       <c r="E4">
-        <f t="shared" ref="E4:E10" si="0">COUNTIF($A$1:$A$47,D4)</f>
-        <v>3</v>
+        <f>D4/SUM($D$1:$D$10)</f>
+        <v>0.25714285714285712</v>
       </c>
       <c r="F4">
-        <f t="shared" ref="F4:F10" si="1">E4/SUM($E$4:$E$13)</f>
-        <v>8.5714285714285715E-2</v>
+        <f>SUM(D$2:D4)</f>
+        <v>23</v>
       </c>
       <c r="G4">
-        <f>SUM(E$4:E4)</f>
-        <v>3</v>
-      </c>
-      <c r="H4">
-        <f>SUM(F$4:F4)</f>
-        <v>8.5714285714285715E-2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+        <f>SUM(E$2:E4)</f>
+        <v>0.65714285714285714</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>9</v>
       </c>
       <c r="B5" s="1">
         <v>5</v>
       </c>
+      <c r="C5">
+        <v>9</v>
+      </c>
       <c r="D5">
-        <v>7</v>
+        <f>COUNTIF($A$1:$A$47,C5)</f>
+        <v>2</v>
       </c>
       <c r="E5">
-        <f t="shared" si="0"/>
-        <v>11</v>
+        <f>D5/SUM($D$1:$D$10)</f>
+        <v>5.7142857142857141E-2</v>
       </c>
       <c r="F5">
-        <f t="shared" si="1"/>
-        <v>0.31428571428571428</v>
+        <f>SUM(D$2:D5)</f>
+        <v>25</v>
       </c>
       <c r="G5">
-        <f>SUM(E$4:E5)</f>
-        <v>14</v>
-      </c>
-      <c r="H5">
-        <f>SUM(F$4:F5)</f>
-        <v>0.4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+        <f>SUM(E$2:E5)</f>
+        <v>0.7142857142857143</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>6</v>
       </c>
       <c r="B6" s="1">
         <v>6</v>
       </c>
+      <c r="C6">
+        <v>10</v>
+      </c>
       <c r="D6">
+        <f>COUNTIF($A$1:$A$47,C6)</f>
         <v>8</v>
       </c>
       <c r="E6">
-        <f t="shared" si="0"/>
-        <v>9</v>
+        <f>D6/SUM($D$1:$D$10)</f>
+        <v>0.22857142857142856</v>
       </c>
       <c r="F6">
-        <f t="shared" si="1"/>
-        <v>0.25714285714285712</v>
+        <f>SUM(D$2:D6)</f>
+        <v>33</v>
       </c>
       <c r="G6">
-        <f>SUM(E$4:E6)</f>
-        <v>23</v>
-      </c>
-      <c r="H6">
-        <f>SUM(F$4:F6)</f>
-        <v>0.65714285714285714</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+        <f>SUM(E$2:E6)</f>
+        <v>0.94285714285714284</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>8</v>
       </c>
       <c r="B7" s="1">
         <v>7</v>
       </c>
+      <c r="C7">
+        <v>11</v>
+      </c>
       <c r="D7">
-        <v>9</v>
+        <f>COUNTIF($A$1:$A$47,C7)</f>
+        <v>2</v>
       </c>
       <c r="E7">
-        <f t="shared" si="0"/>
-        <v>2</v>
+        <f>D7/SUM($D$1:$D$10)</f>
+        <v>5.7142857142857141E-2</v>
       </c>
       <c r="F7">
-        <f t="shared" si="1"/>
-        <v>5.7142857142857141E-2</v>
+        <f>SUM(D$2:D7)</f>
+        <v>35</v>
       </c>
       <c r="G7">
-        <f>SUM(E$4:E7)</f>
-        <v>25</v>
-      </c>
-      <c r="H7">
-        <f>SUM(F$4:F7)</f>
-        <v>0.7142857142857143</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+        <f>SUM(E$2:E7)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" s="1">
         <v>8</v>
       </c>
+      <c r="C8">
+        <v>12</v>
+      </c>
       <c r="D8">
-        <v>10</v>
+        <f>COUNTIF($A$1:$A$47,C8)</f>
+        <v>0</v>
       </c>
       <c r="E8">
-        <f t="shared" si="0"/>
-        <v>8</v>
+        <f>D8/SUM($D$1:$D$10)</f>
+        <v>0</v>
       </c>
       <c r="F8">
-        <f t="shared" si="1"/>
-        <v>0.22857142857142856</v>
+        <f>SUM(D$2:D8)</f>
+        <v>35</v>
       </c>
       <c r="G8">
-        <f>SUM(E$4:E8)</f>
-        <v>33</v>
-      </c>
-      <c r="H8">
-        <f>SUM(F$4:F8)</f>
-        <v>0.94285714285714284</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+        <f>SUM(E$2:E8)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>7</v>
       </c>
       <c r="B9" s="1">
         <v>9</v>
       </c>
-      <c r="D9">
-        <v>11</v>
-      </c>
-      <c r="E9">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="F9">
-        <f t="shared" si="1"/>
-        <v>5.7142857142857141E-2</v>
-      </c>
-      <c r="G9">
-        <f>SUM(E$4:E9)</f>
-        <v>35</v>
-      </c>
-      <c r="H9">
-        <f>SUM(F$4:F9)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>10</v>
       </c>
       <c r="B10" s="1">
         <v>10</v>
       </c>
-      <c r="D10">
-        <v>12</v>
-      </c>
-      <c r="E10">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F10">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="G10">
-        <f>SUM(E$4:E10)</f>
-        <v>35</v>
-      </c>
-      <c r="H10">
-        <f>SUM(F$4:F10)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1666,7 +1676,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>7</v>
       </c>
@@ -1674,7 +1684,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>8</v>
       </c>
@@ -1682,7 +1692,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>7</v>
       </c>
@@ -1690,7 +1700,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>10</v>
       </c>
@@ -1698,7 +1708,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>8</v>
       </c>
@@ -1955,6 +1965,7 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
   <drawing r:id="rId1"/>

</xml_diff>